<commit_message>
modified:   Jupyter scripts/main.ipynb 	modified:   Libaries/__pycache__/sensitivity.cpython-311.pyc 	modified:   Libaries/sensitivity.py 	modified:   data/database.xlsx 	modified:   data/temp.xlsx 	modified:   results/LCIA/LCIA_results.xlsx 	modified:   results/LCIA/LCIA_results_uniquie.xlsx 	modified:   results/figures/monte_carlo.png 	modified:   results/figures/senstivity.png 	modified:   results/sensitivity/penincillium_G.xlsx 	modified:   results/sensitivity/penincillium_V.xlsx
</commit_message>
<xml_diff>
--- a/results/LCIA/LCIA_results.xlsx
+++ b/results/LCIA/LCIA_results.xlsx
@@ -85,130 +85,130 @@
     <t>Penicillin V, Defined daily dose</t>
   </si>
   <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.03687377350639722, "'full box of vials' (unit, NO, None)": 0.002438811269004143, "'production of gloves' (unit, MY, None)": 2.5487657719362628e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0002160601095711479, "'production of IV sets' (unit, RER, None)": 0.007510064787632834, "'medical connector' (unit, GLO, None)": 0.0017344477131681203, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.8090856463642605e-08, "'stopcock' (unit, GLO, None)": 0.0013791234080418571, "'market for water, ultrapure' (kilogram, RER, None)": 2.826776424295117e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0001239026682776555}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.0951510731399976e-05, "'packed box of penicillin' (unit, SE, None)": 0.0008129370896680477, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -6.708351511736244e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 9.157606061618091, "'full box of vials' (unit, NO, None)": 0.6797642657932736, "'production of gloves' (unit, MY, None)": 0.007824541303926095, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.043977797442494006, "'production of IV sets' (unit, RER, None)": 2.6021887356279105, "'medical connector' (unit, GLO, None)": 0.6079081935896292, "'market for sodium chlorate, powder' (kilogram, RER, None)": 5.482256131159481e-06, "'stopcock' (unit, GLO, None)": 0.3212348689127178, "'market for water, ultrapure' (kilogram, RER, None)": 0.00972956859064599, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.15039954351287288}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0027198090003005735, "'packed box of penicillin' (unit, SE, None)": 0.22658808859775792, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.0594192711933484e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.1027289922082144, "'full box of vials' (unit, NO, None)": 0.05388705068225301, "'production of gloves' (unit, MY, None)": 0.000337432919605203, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.009995236525857041, "'production of IV sets' (unit, RER, None)": 0.1359491112893313, "'medical connector' (unit, GLO, None)": 0.018047960158005204, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.8204624103297398e-07, "'stopcock' (unit, GLO, None)": 0.012492779924667078, "'market for water, ultrapure' (kilogram, RER, None)": 0.00033203580675661166, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0025378130132093627}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.00032751051068583974, "'packed box of penicillin' (unit, SE, None)": 0.01796235022741767, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -8.881234444008943e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.5745809800413217, "'full box of vials' (unit, NO, None)": 0.07095240600829245, "'production of gloves' (unit, MY, None)": 0.0004496893111358022, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.014788492908451925, "'production of IV sets' (unit, RER, None)": 0.16855450425410312, "'medical connector' (unit, GLO, None)": 0.023746812174586407, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.416887787840655e-07, "'stopcock' (unit, GLO, None)": 0.01689608276567772, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004282569023378724, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.003462826564810457}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0004676505510722726, "'packed box of penicillin' (unit, SE, None)": 0.023650802002764152, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.1835822669094316e-06}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 56.83593116548929, "'full box of vials' (unit, NO, None)": 2.6454328532142863, "'production of gloves' (unit, MY, None)": 0.016607272715656627, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.360667253371816, "'production of IV sets' (unit, RER, None)": 11.566964195939653, "'medical connector' (unit, GLO, None)": 1.6751475067156671, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.7715337048192276e-05, "'stopcock' (unit, GLO, None)": 1.1501230564879843, "'market for water, ultrapure' (kilogram, RER, None)": 0.03075217754184183, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.13862157733378083}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.016880271556150322, "'packed box of penicillin' (unit, SE, None)": 0.8818109510714289, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.371034178760824e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 2.4760114102259623, "'full box of vials' (unit, NO, None)": 0.1821712711072902, "'production of gloves' (unit, MY, None)": 0.002018020334749927, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.012725749065683542, "'production of IV sets' (unit, RER, None)": 0.6837967361585064, "'medical connector' (unit, GLO, None)": 0.28547008943019353, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.452139893165589e-06, "'stopcock' (unit, GLO, None)": 0.16565150319386726, "'market for water, ultrapure' (kilogram, RER, None)": 0.004298967286016907, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.015032573624970104}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.000735375388837111, "'packed box of penicillin' (unit, SE, None)": 0.06072375703576341, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.3114295210618075e-06}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.003483205819891305, "'full box of vials' (unit, NO, None)": 0.0005747426092024944, "'production of gloves' (unit, MY, None)": 0.00014021999691295897, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 2.489813809894416e-05, "'production of IV sets' (unit, RER, None)": 0.0007085002074647097, "'medical connector' (unit, GLO, None)": 0.00015211175147422895, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.000069133869748e-09, "'stopcock' (unit, GLO, None)": 8.074128794356362e-05, "'market for water, ultrapure' (kilogram, RER, None)": 2.7329978977877557e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.1034569967112516e-05}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.0345121285077176e-06, "'packed box of penicillin' (unit, SE, None)": 0.0001915808697341648, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.6905903187490804e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.0010037883972532416, "'full box of vials' (unit, NO, None)": 6.2464613468254e-05, "'production of gloves' (unit, MY, None)": 1.921109637292979e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.4053438864662445e-06, "'production of IV sets' (unit, RER, None)": 0.0005893145726141097, "'medical connector' (unit, GLO, None)": 2.0791331489972104e-05, "'market for sodium chlorate, powder' (kilogram, RER, None)": 7.53113354539674e-10, "'stopcock' (unit, GLO, None)": 1.89138817186539e-05, "'market for water, ultrapure' (kilogram, RER, None)": 3.2219775859022905e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.259501398776277e-06}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 2.981251539842128e-07, "'packed box of penicillin' (unit, SE, None)": 2.0821537822751333e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.056360565355121e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.0085092464862693, "'full box of vials' (unit, NO, None)": 0.1293826461137576, "'production of gloves' (unit, MY, None)": 0.00163727486533218, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.006987260151454363, "'production of IV sets' (unit, RER, None)": 0.11385661981675224, "'medical connector' (unit, GLO, None)": 0.027135028072205268, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.42638688178418e-07, "'stopcock' (unit, GLO, None)": 0.016910083754528685, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004616459876258445, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.016495414906957998}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.00029952724620642196, "'packed box of penicillin' (unit, SE, None)": 0.04312754870458588, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.309307445554298e-06}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 19.124255465019452, "'full box of vials' (unit, NO, None)": 1.2322214079751332, "'production of gloves' (unit, MY, None)": 0.00905512597768007, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.17590535184680844, "'production of IV sets' (unit, RER, None)": 2.188784540613683, "'medical connector' (unit, GLO, None)": 0.39938174456537434, "'market for sodium chlorate, powder' (kilogram, RER, None)": 5.148719601293815e-06, "'stopcock' (unit, GLO, None)": 0.3250128429457947, "'market for water, ultrapure' (kilogram, RER, None)": 0.007121871856965159, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.05951396844437705}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.005679903873110778, "'packed box of penicillin' (unit, SE, None)": 0.4107404693250445, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.3833091573253948e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.9543242997057164, "'full box of vials' (unit, NO, None)": 0.3571104943760466, "'production of gloves' (unit, MY, None)": 0.003970447074241809, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0018484501766666355, "'production of IV sets' (unit, RER, None)": 0.20871337205959184, "'medical connector' (unit, GLO, None)": 0.035517690500554644, "'market for sodium chlorate, powder' (kilogram, RER, None)": 4.1827803179068245e-07, "'stopcock' (unit, GLO, None)": 0.021417644848113586, "'market for water, ultrapure' (kilogram, RER, None)": 0.000615362580615432, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.002230303873870607}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0002834343170125978, "'packed box of penicillin' (unit, SE, None)": 0.11903683145868221, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.0450216699404443e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.886700903000281, "'full box of vials' (unit, NO, None)": 0.021760828160990366, "'production of gloves' (unit, MY, None)": 0.00021512651686035866, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0009482808379063375, "'production of IV sets' (unit, RER, None)": 0.33259128836154267, "'medical connector' (unit, GLO, None)": 0.018670347067374398, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.9288147257864155e-06, "'stopcock' (unit, GLO, None)": 0.03007979304831096, "'market for water, ultrapure' (kilogram, RER, None)": 0.00021113544250004932, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0005977399525779672}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0002633501681910835, "'packed box of penicillin' (unit, SE, None)": 0.007253609386996789, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.66212992376464e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.25416546117760835, "'full box of vials' (unit, NO, None)": 0.04077816330719616, "'production of gloves' (unit, MY, None)": 0.0002092993481978399, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0014445867303929784, "'production of IV sets' (unit, RER, None)": 0.06299082557386283, "'medical connector' (unit, GLO, None)": 0.014656755286088938, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.6809075379619639e-06, "'stopcock' (unit, GLO, None)": 0.0230986742704935, "'market for water, ultrapure' (kilogram, RER, None)": 0.0001664766728635228, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0023610768777571497}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 7.54871419697497e-05, "'packed box of penicillin' (unit, SE, None)": 0.01359272110239872, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.508758844567146e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 4.5315639414904654e-06, "'full box of vials' (unit, NO, None)": 3.191488205692017e-07, "'production of gloves' (unit, MY, None)": 3.834203679632982e-09, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.2070601951951626e-08, "'production of IV sets' (unit, RER, None)": 3.4392664008051865e-06, "'medical connector' (unit, GLO, None)": 1.83276723357176e-07, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.2306374543392183e-12, "'stopcock' (unit, GLO, None)": 9.16973660450892e-08, "'market for water, ultrapure' (kilogram, RER, None)": 2.480877864385071e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.98928318147166e-08}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.3458744906226682e-09, "'packed box of penicillin' (unit, SE, None)": 1.063829401897339e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.0091624084794008e-11}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.01570647054979859, "'full box of vials' (unit, NO, None)": 0.0009952287948037596, "'production of gloves' (unit, MY, None)": 1.0564784242098315e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 9.323734263665946e-05, "'production of IV sets' (unit, RER, None)": 0.0028193371897081657, "'medical connector' (unit, GLO, None)": 0.0007940185977603063, "'market for sodium chlorate, powder' (kilogram, RER, None)": 9.087066473931986e-09, "'stopcock' (unit, GLO, None)": 0.0005910881849974128, "'market for water, ultrapure' (kilogram, RER, None)": 1.3611427406045218e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.6633047758711216e-05}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 4.664821753290181e-06, "'packed box of penicillin' (unit, SE, None)": 0.0003317429316012532, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.7806512125202764e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.028468239812098402, "'full box of vials' (unit, NO, None)": 0.0013267250993028426, "'production of gloves' (unit, MY, None)": 1.4163531981861828e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00013038775065437092, "'production of IV sets' (unit, RER, None)": 0.005326359857987854, "'medical connector' (unit, GLO, None)": 0.0013055374310446998, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.43133039828799e-08, "'stopcock' (unit, GLO, None)": 0.0012081588968752607, "'market for water, ultrapure' (kilogram, RER, None)": 2.148282919471022e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011138873801415913}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 8.455067224193225e-06, "'packed box of penicillin' (unit, SE, None)": 0.00044224169976761425, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.727841617626033e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.029319164480471484, "'full box of vials' (unit, NO, None)": 0.001370266892586484, "'production of gloves' (unit, MY, None)": 1.4684860725651736e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00013398816811632376, "'production of IV sets' (unit, RER, None)": 0.005619212119632552, "'medical connector' (unit, GLO, None)": 0.001387442899209297, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.5185667755584578e-08, "'stopcock' (unit, GLO, None)": 0.001295257516709964, "'market for water, ultrapure' (kilogram, RER, None)": 2.3010588474039736e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011945921291183066}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 8.707791850700031e-06, "'packed box of penicillin' (unit, SE, None)": 0.00045675563086216143, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.865055342991537e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.09846959749397198, "'full box of vials' (unit, NO, None)": 0.0360019241349114, "'production of gloves' (unit, MY, None)": 0.00031739329180492616, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00043001785193021565, "'production of IV sets' (unit, RER, None)": 0.06341294965705647, "'medical connector' (unit, GLO, None)": 0.006814612420672324, "'market for sodium chlorate, powder' (kilogram, RER, None)": 8.352207093722833e-08, "'stopcock' (unit, GLO, None)": 0.00458831520443211, "'market for water, ultrapure' (kilogram, RER, None)": 0.00011038760143956678, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.000510308361458836}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 2.924547045570968e-05, "'packed box of penicillin' (unit, SE, None)": 0.012000641378303801, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -8.353791440305657e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 4.9024541089205705e-08, "'full box of vials' (unit, NO, None)": 3.250424631822603e-09, "'production of gloves' (unit, MY, None)": 1.2552595632407548e-10, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 2.2394391948019352e-10, "'production of IV sets' (unit, RER, None)": 1.3275643024918078e-08, "'medical connector' (unit, GLO, None)": 2.551022562941903e-09, "'market for sodium chlorate, powder' (kilogram, RER, None)": 3.9947793408828877e-14, "'stopcock' (unit, GLO, None)": 1.7036204046426842e-09, "'market for water, ultrapure' (kilogram, RER, None)": 4.054206389503784e-11, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.993349475283916e-10}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.4560288703494096e-11, "'packed box of penicillin' (unit, SE, None)": 1.083474877274201e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.3038431704496666e-13}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 2.6331989940519182e-05, "'full box of vials' (unit, NO, None)": 2.050867904215491e-06, "'production of gloves' (unit, MY, None)": 2.2151400772758927e-08, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.637969189098489e-07, "'production of IV sets' (unit, RER, None)": 5.212872849674814e-06, "'medical connector' (unit, GLO, None)": 1.2608984822087683e-06, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.2980902016512886e-11, "'stopcock' (unit, GLO, None)": 8.112728106451089e-07, "'market for water, ultrapure' (kilogram, RER, None)": 2.100937926796612e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.4476941816577837e-07}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 7.820601012334199e-09, "'packed box of penicillin' (unit, SE, None)": 6.836226347384971e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.83024868339015e-11}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.7961888513131341, "'full box of vials' (unit, NO, None)": 0.048278799751043315, "'production of gloves' (unit, MY, None)": 0.00047405600821686636, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.003773742559756964, "'production of IV sets' (unit, RER, None)": 0.2386394669772794, "'medical connector' (unit, GLO, None)": 0.10451083709719641, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.2485945719127488e-06, "'stopcock' (unit, GLO, None)": 0.0686053832681468, "'market for water, ultrapure' (kilogram, RER, None)": 0.0015021057998050832, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.006191267786717013}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.00023646808884000083, "'packed box of penicillin' (unit, SE, None)": 0.01609293325034777, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.2477154136267921e-06}</t>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.03687599128885077, "'full box of vials' (unit, NO, None)": 0.002438811219158838, "'production of gloves' (unit, MY, None)": 2.5487655181193988e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00021606011111678373, "'production of IV sets' (unit, RER, None)": 0.007513724073311152, "'medical connector' (unit, GLO, None)": 0.0017344477281822704, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.809085650704119e-08, "'stopcock' (unit, GLO, None)": 0.001379123421163791, "'market for water, ultrapure' (kilogram, RER, None)": 2.82677643401405e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00012390267267150542}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.095216941278868e-05, "'packed box of penicillin' (unit, SE, None)": 0.0008129370730529461, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -6.708350843690258e-08}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 9.15819746391152, "'full box of vials' (unit, NO, None)": 0.6797642589426867, "'production of gloves' (unit, MY, None)": 0.007824541001041022, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.04397779769519084, "'production of IV sets' (unit, RER, None)": 2.6031645089523616, "'medical connector' (unit, GLO, None)": 0.6079081961884432, "'market for sodium chlorate, powder' (kilogram, RER, None)": 5.4822561328596534e-06, "'stopcock' (unit, GLO, None)": 0.3212348706867777, "'market for water, ultrapure' (kilogram, RER, None)": 0.009729568609049168, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.15039954374451905}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.002719984646781722, "'packed box of penicillin' (unit, SE, None)": 0.2265880863142289, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.0594191914739972e-05}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.1027918266733838, "'full box of vials' (unit, NO, None)": 0.05388704819491359, "'production of gloves' (unit, MY, None)": 0.0003374327632707171, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.009995236595088717, "'production of IV sets' (unit, RER, None)": 0.13605279430910955, "'medical connector' (unit, GLO, None)": 0.018047960751005683, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.8204624235459882e-07, "'stopcock' (unit, GLO, None)": 0.012492780408536224, "'market for water, ultrapure' (kilogram, RER, None)": 0.00033203580697507915, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0025378132414232233}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.000327529172521995, "'packed box of penicillin' (unit, SE, None)": 0.01796234939830453, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -8.881230329285274e-07}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.5746661470927679, "'full box of vials' (unit, NO, None)": 0.07095240280146164, "'production of gloves' (unit, MY, None)": 0.00044968911016173864, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.01478849299863757, "'production of IV sets' (unit, RER, None)": 0.1686950375460201, "'medical connector' (unit, GLO, None)": 0.023746812954197526, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.416887805880026e-07, "'stopcock' (unit, GLO, None)": 0.016896083394812668, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004282569029177262, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0034628268610128335}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0004676758456865521, "'packed box of penicillin' (unit, SE, None)": 0.023650800933820552, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.1835817379456963e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 56.839779366368276, "'full box of vials' (unit, NO, None)": 2.6454326399879715, "'production of gloves' (unit, MY, None)": 0.016607258349745812, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.3606672604604086, "'production of IV sets' (unit, RER, None)": 11.573314103223865, "'medical connector' (unit, GLO, None)": 1.6751475800286304, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.7715337264655672e-05, "'stopcock' (unit, GLO, None)": 1.150123107100565, "'market for water, ultrapure' (kilogram, RER, None)": 0.03075217784152998, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.13862159996276088}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.01688141447181138, "'packed box of penicillin' (unit, SE, None)": 0.8818108799959905, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.371030397653098e-05}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 2.4761450202313835, "'full box of vials' (unit, NO, None)": 0.18217126914294418, "'production of gloves' (unit, MY, None)": 0.0020180202531192015, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.012725749116188194, "'production of IV sets' (unit, RER, None)": 0.6840171844921856, "'medical connector' (unit, GLO, None)": 0.2854700899924798, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.4521398891490502e-06, "'stopcock' (unit, GLO, None)": 0.1656515035528201, "'market for water, ultrapure' (kilogram, RER, None)": 0.004298967287758422, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.015032573610983896}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0007354150710087209, "'packed box of penicillin' (unit, SE, None)": 0.0607237563809814, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.311429306209739e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.003486442859530362, "'full box of vials' (unit, NO, None)": 0.0005747426059833386, "'production of gloves' (unit, MY, None)": 0.0001402199966880572, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 2.4898138270273555e-05, "'production of IV sets' (unit, RER, None)": 0.0007138413112786659, "'medical connector' (unit, GLO, None)": 0.00015211175360090154, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.000069144812745e-09, "'stopcock' (unit, GLO, None)": 8.074128916414129e-05, "'market for water, ultrapure' (kilogram, RER, None)": 2.73299791267522e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.103457038626477e-05}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.0354735292805177e-06, "'packed box of penicillin' (unit, SE, None)": 0.0001915808686611129, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.690590312829666e-07}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.0010147729344861668, "'full box of vials' (unit, NO, None)": 6.246461306720517e-05, "'production of gloves' (unit, MY, None)": 1.921109635646681e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.4053438981334531e-06, "'production of IV sets' (unit, RER, None)": 0.0006074390570590995, "'medical connector' (unit, GLO, None)": 2.079133161330272e-05, "'market for sodium chlorate, powder' (kilogram, RER, None)": 7.531133548021007e-10, "'stopcock' (unit, GLO, None)": 1.8913881794348918e-05, "'market for water, ultrapure' (kilogram, RER, None)": 3.22197759040506e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.259501418017439e-06}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 3.013875615423916e-07, "'packed box of penicillin' (unit, SE, None)": 2.0821537689068392e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.056360561022065e-08}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.008614349969602, "'full box of vials' (unit, NO, None)": 0.12938264326667515, "'production of gloves' (unit, MY, None)": 0.0016372747483247695, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0069872602674408285, "'production of IV sets' (unit, RER, None)": 0.11403002376828243, "'medical connector' (unit, GLO, None)": 0.027135029208152847, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.426386943287326e-07, "'stopcock' (unit, GLO, None)": 0.016910084457867687, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004616459876020485, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.016495415120892556}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.00029955846194097186, "'packed box of penicillin' (unit, SE, None)": 0.04312754775555839, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.309307137590793e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 19.130447432366296, "'full box of vials' (unit, NO, None)": 1.2322213718268222, "'production of gloves' (unit, MY, None)": 0.009055123633314255, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.17590535300444554, "'production of IV sets' (unit, RER, None)": 2.1990013469576892, "'medical connector' (unit, GLO, None)": 0.39938175571307044, "'market for sodium chlorate, powder' (kilogram, RER, None)": 5.148719634703583e-06, "'stopcock' (unit, GLO, None)": 0.3250128508974576, "'market for water, ultrapure' (kilogram, RER, None)": 0.0071218718989447885, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.059513972203317125}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.005681742887412791, "'packed box of penicillin' (unit, SE, None)": 0.4107404572756075, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.383308540288312e-05}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.9544240647015759, "'full box of vials' (unit, NO, None)": 0.3571104942253917, "'production of gloves' (unit, MY, None)": 0.00397044706317054, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0018484501955930203, "'production of IV sets' (unit, RER, None)": 0.20887798199967178, "'medical connector' (unit, GLO, None)": 0.03551769074884779, "'market for sodium chlorate, powder' (kilogram, RER, None)": 4.1827803350125506e-07, "'stopcock' (unit, GLO, None)": 0.02141764497794181, "'market for water, ultrapure' (kilogram, RER, None)": 0.0006153625812945318, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00223030389672603}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0002834639472163681, "'packed box of penicillin' (unit, SE, None)": 0.11903683140846391, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.0450216670264861e-05}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.8867178454987492, "'full box of vials' (unit, NO, None)": 0.02176082778009882, "'production of gloves' (unit, MY, None)": 0.00021512640371472653, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.000948280859940274, "'production of IV sets' (unit, RER, None)": 0.33261922330544524, "'medical connector' (unit, GLO, None)": 0.018670347089575857, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.9288147293366414e-06, "'stopcock' (unit, GLO, None)": 0.030079793081911083, "'market for water, ultrapure' (kilogram, RER, None)": 0.00021113546013968885, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0005977400582210082}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.00026335520011312854, "'packed box of penicillin' (unit, SE, None)": 0.00725360926003294, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.662126945771603e-07}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.25418916593008745, "'full box of vials' (unit, NO, None)": 0.040778162362854455, "'production of gloves' (unit, MY, None)": 0.00020929931702298992, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.001444586756887401, "'production of IV sets' (unit, RER, None)": 0.06302993413100622, "'medical connector' (unit, GLO, None)": 0.01465675552791771, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.6809075394952411e-06, "'stopcock' (unit, GLO, None)": 0.02309867442366211, "'market for water, ultrapure' (kilogram, RER, None)": 0.00016647667404630034, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.002361076938021631}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 7.549418228123598e-05, "'packed box of penicillin' (unit, SE, None)": 0.013592720787618152, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.508758024045095e-07}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 4.534613583951555e-06, "'full box of vials' (unit, NO, None)": 3.1914881829874047e-07, "'production of gloves' (unit, MY, None)": 3.8342036009936194e-09, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.2070602024453945e-08, "'production of IV sets' (unit, RER, None)": 3.4442983011362307e-06, "'medical connector' (unit, GLO, None)": 1.832767242754516e-07, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.2306374555740777e-12, "'stopcock' (unit, GLO, None)": 9.169736687692799e-08, "'market for water, ultrapure' (kilogram, RER, None)": 2.480877871327275e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.989283198447722e-08}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.346780234433612e-09, "'packed box of penicillin' (unit, SE, None)": 1.0638293943291351e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.0091623877815206e-11}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.01570731896700782, "'full box of vials' (unit, NO, None)": 0.0009952287770433926, "'production of gloves' (unit, MY, None)": 1.0564783297296858e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 9.323734333854125e-05, "'production of IV sets' (unit, RER, None)": 0.002820737018573794, "'medical connector' (unit, GLO, None)": 0.0007940186047471415, "'market for sodium chlorate, powder' (kilogram, RER, None)": 9.087066504422402e-09, "'stopcock' (unit, GLO, None)": 0.0005910881915482605, "'market for water, ultrapure' (kilogram, RER, None)": 1.3611427443396664e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.663304958430372e-05}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 4.6650737332013236e-06, "'packed box of penicillin' (unit, SE, None)": 0.0003317429256811309, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.780650963848533e-08}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.028469902593481512, "'full box of vials' (unit, NO, None)": 0.0013267250712529284, "'production of gloves' (unit, MY, None)": 1.4163530975786153e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00013038775144206985, "'production of IV sets' (unit, RER, None)": 0.005329103349090954, "'medical connector' (unit, GLO, None)": 0.0013055374386428968, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.4313303962684281e-08, "'stopcock' (unit, GLO, None)": 0.0012081589085005972, "'market for water, ultrapure' (kilogram, RER, None)": 2.1482829273697714e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011138873995824629}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 8.45556107026401e-06, "'packed box of penicillin' (unit, SE, None)": 0.0004422416904176429, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.727841352826915e-08}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.029320884509801824, "'full box of vials' (unit, NO, None)": 0.001370266861425661, "'production of gloves' (unit, MY, None)": 1.4684859631314947e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00013398816890110104, "'production of IV sets' (unit, RER, None)": 0.0056220500711255126, "'medical connector' (unit, GLO, None)": 0.0013874429068758327, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.5185667717271498e-08, "'stopcock' (unit, GLO, None)": 0.00129525752812853, "'market for water, ultrapure' (kilogram, RER, None)": 2.301058855254493e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011945921458723627}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 8.708302699411142e-06, "'packed box of penicillin' (unit, SE, None)": 0.00045675562047522034, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.865055054962094e-08}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.0984780181258722, "'full box of vials' (unit, NO, None)": 0.03600192407055957, "'production of gloves' (unit, MY, None)": 0.0003173932895559447, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0004300178534555128, "'production of IV sets' (unit, RER, None)": 0.06342684359841966, "'medical connector' (unit, GLO, None)": 0.006814612431333982, "'market for sodium chlorate, powder' (kilogram, RER, None)": 8.352207092016413e-08, "'stopcock' (unit, GLO, None)": 0.0045883152102746995, "'market for water, ultrapure' (kilogram, RER, None)": 0.00011038760144267684, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0005103083642199823}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 2.924797138338405e-05, "'packed box of penicillin' (unit, SE, None)": 0.01200064135685319, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -8.353791381112465e-07}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 4.902932398442658e-08, "'full box of vials' (unit, NO, None)": 3.250424588023479e-09, "'production of gloves' (unit, MY, None)": 1.255259533483824e-10, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 2.2394392106546851e-10, "'production of IV sets' (unit, RER, None)": 1.3283534486921163e-08, "'medical connector' (unit, GLO, None)": 2.5510225773413464e-09, "'market for sodium chlorate, powder' (kilogram, RER, None)": 3.994779346027959e-14, "'stopcock' (unit, GLO, None)": 1.7036204159597961e-09, "'market for water, ultrapure' (kilogram, RER, None)": 4.054206414751791e-11, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.99334950990401e-10}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.4561709223374696e-11, "'packed box of penicillin' (unit, SE, None)": 1.083474862674493e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.303843092129425e-13}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 2.633485617414525e-05, "'full box of vials' (unit, NO, None)": 2.050867868836324e-06, "'production of gloves' (unit, MY, None)": 2.215139896920989e-08, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.6379692023869563e-07, "'production of IV sets' (unit, RER, None)": 5.217602017801188e-06, "'medical connector' (unit, GLO, None)": 1.2608984953567032e-06, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.2980902065251225e-11, "'stopcock' (unit, GLO, None)": 8.112728205819187e-07, "'market for water, ultrapure' (kilogram, RER, None)": 2.1009379318096128e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.4476942110326793e-07}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 7.82145228372114e-09, "'packed box of penicillin' (unit, SE, None)": 6.836226229454415e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.830248208696044e-11}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.7962346041941827, "'full box of vials' (unit, NO, None)": 0.048278798871591394, "'production of gloves' (unit, MY, None)": 0.00047405597484428193, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0037737425754329895, "'production of IV sets' (unit, RER, None)": 0.23871495679333327, "'medical connector' (unit, GLO, None)": 0.10451083724522091, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.2485945693722554e-06, "'stopcock' (unit, GLO, None)": 0.06860538337334873, "'market for water, ultrapure' (kilogram, RER, None)": 0.0015021057997467893, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.006191267771795764}</t>
+  </si>
+  <si>
+    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0002364816774456723, "'packed box of penicillin' (unit, SE, None)": 0.01609293295719713, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.2477153257901502e-06}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
modified:   Jupyter scripts/main.ipynb 	modified:   Jupyter scripts/playground.ipynb 	new file:   Libaries/__pycache__/lcia_results_copy.cpython-311.pyc 	modified:   Libaries/__pycache__/sensitivity.cpython-311.pyc 	new file:   Libaries/lcia_results_copy.py 	modified:   data/database.xlsx 	modified:   data/temp.xlsx 	modified:   results/LCIA/LCIA_results.xlsx 	new file:   results/LCIA/LCIA_results_unique.xlsx 	modified:   results/LCIA/LCIA_results_uniquie.xlsx 	modified:   results/figures/endpoint (H).png 	modified:   results/figures/midpoint (H).png 	modified:   results/figures/monte_carlo.png 	modified:   results/figures/senstivity.png 	modified:   results/sensitivity/penincillium_G.xlsx 	modified:   results/sensitivity/penincillium_V.xlsx
</commit_message>
<xml_diff>
--- a/results/LCIA/LCIA_results.xlsx
+++ b/results/LCIA/LCIA_results.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="penicillin" sheetId="1" r:id="rId1"/>
+    <sheet name="penicillin_cut_off" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -85,130 +85,130 @@
     <t>Penicillin V, Defined daily dose</t>
   </si>
   <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.03687599128885077, "'full box of vials' (unit, NO, None)": 0.002438811219158838, "'production of gloves' (unit, MY, None)": 2.5487655181193988e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00021606011111678373, "'production of IV sets' (unit, RER, None)": 0.007513724073311152, "'medical connector' (unit, GLO, None)": 0.0017344477281822704, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.809085650704119e-08, "'stopcock' (unit, GLO, None)": 0.001379123421163791, "'market for water, ultrapure' (kilogram, RER, None)": 2.82677643401405e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00012390267267150542}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.095216941278868e-05, "'packed box of penicillin' (unit, SE, None)": 0.0008129370730529461, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -6.708350843690258e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 9.15819746391152, "'full box of vials' (unit, NO, None)": 0.6797642589426867, "'production of gloves' (unit, MY, None)": 0.007824541001041022, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.04397779769519084, "'production of IV sets' (unit, RER, None)": 2.6031645089523616, "'medical connector' (unit, GLO, None)": 0.6079081961884432, "'market for sodium chlorate, powder' (kilogram, RER, None)": 5.4822561328596534e-06, "'stopcock' (unit, GLO, None)": 0.3212348706867777, "'market for water, ultrapure' (kilogram, RER, None)": 0.009729568609049168, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.15039954374451905}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.002719984646781722, "'packed box of penicillin' (unit, SE, None)": 0.2265880863142289, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.0594191914739972e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.1027918266733838, "'full box of vials' (unit, NO, None)": 0.05388704819491359, "'production of gloves' (unit, MY, None)": 0.0003374327632707171, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.009995236595088717, "'production of IV sets' (unit, RER, None)": 0.13605279430910955, "'medical connector' (unit, GLO, None)": 0.018047960751005683, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.8204624235459882e-07, "'stopcock' (unit, GLO, None)": 0.012492780408536224, "'market for water, ultrapure' (kilogram, RER, None)": 0.00033203580697507915, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0025378132414232233}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.000327529172521995, "'packed box of penicillin' (unit, SE, None)": 0.01796234939830453, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -8.881230329285274e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.5746661470927679, "'full box of vials' (unit, NO, None)": 0.07095240280146164, "'production of gloves' (unit, MY, None)": 0.00044968911016173864, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.01478849299863757, "'production of IV sets' (unit, RER, None)": 0.1686950375460201, "'medical connector' (unit, GLO, None)": 0.023746812954197526, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.416887805880026e-07, "'stopcock' (unit, GLO, None)": 0.016896083394812668, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004282569029177262, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0034628268610128335}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0004676758456865521, "'packed box of penicillin' (unit, SE, None)": 0.023650800933820552, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.1835817379456963e-06}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 56.839779366368276, "'full box of vials' (unit, NO, None)": 2.6454326399879715, "'production of gloves' (unit, MY, None)": 0.016607258349745812, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.3606672604604086, "'production of IV sets' (unit, RER, None)": 11.573314103223865, "'medical connector' (unit, GLO, None)": 1.6751475800286304, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.7715337264655672e-05, "'stopcock' (unit, GLO, None)": 1.150123107100565, "'market for water, ultrapure' (kilogram, RER, None)": 0.03075217784152998, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.13862159996276088}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.01688141447181138, "'packed box of penicillin' (unit, SE, None)": 0.8818108799959905, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.371030397653098e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 2.4761450202313835, "'full box of vials' (unit, NO, None)": 0.18217126914294418, "'production of gloves' (unit, MY, None)": 0.0020180202531192015, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.012725749116188194, "'production of IV sets' (unit, RER, None)": 0.6840171844921856, "'medical connector' (unit, GLO, None)": 0.2854700899924798, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.4521398891490502e-06, "'stopcock' (unit, GLO, None)": 0.1656515035528201, "'market for water, ultrapure' (kilogram, RER, None)": 0.004298967287758422, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.015032573610983896}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0007354150710087209, "'packed box of penicillin' (unit, SE, None)": 0.0607237563809814, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.311429306209739e-06}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.003486442859530362, "'full box of vials' (unit, NO, None)": 0.0005747426059833386, "'production of gloves' (unit, MY, None)": 0.0001402199966880572, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 2.4898138270273555e-05, "'production of IV sets' (unit, RER, None)": 0.0007138413112786659, "'medical connector' (unit, GLO, None)": 0.00015211175360090154, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.000069144812745e-09, "'stopcock' (unit, GLO, None)": 8.074128916414129e-05, "'market for water, ultrapure' (kilogram, RER, None)": 2.73299791267522e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.103457038626477e-05}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.0354735292805177e-06, "'packed box of penicillin' (unit, SE, None)": 0.0001915808686611129, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.690590312829666e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.0010147729344861668, "'full box of vials' (unit, NO, None)": 6.246461306720517e-05, "'production of gloves' (unit, MY, None)": 1.921109635646681e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.4053438981334531e-06, "'production of IV sets' (unit, RER, None)": 0.0006074390570590995, "'medical connector' (unit, GLO, None)": 2.079133161330272e-05, "'market for sodium chlorate, powder' (kilogram, RER, None)": 7.531133548021007e-10, "'stopcock' (unit, GLO, None)": 1.8913881794348918e-05, "'market for water, ultrapure' (kilogram, RER, None)": 3.22197759040506e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.259501418017439e-06}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 3.013875615423916e-07, "'packed box of penicillin' (unit, SE, None)": 2.0821537689068392e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.056360561022065e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.008614349969602, "'full box of vials' (unit, NO, None)": 0.12938264326667515, "'production of gloves' (unit, MY, None)": 0.0016372747483247695, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0069872602674408285, "'production of IV sets' (unit, RER, None)": 0.11403002376828243, "'medical connector' (unit, GLO, None)": 0.027135029208152847, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.426386943287326e-07, "'stopcock' (unit, GLO, None)": 0.016910084457867687, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004616459876020485, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.016495415120892556}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.00029955846194097186, "'packed box of penicillin' (unit, SE, None)": 0.04312754775555839, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.309307137590793e-06}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 19.130447432366296, "'full box of vials' (unit, NO, None)": 1.2322213718268222, "'production of gloves' (unit, MY, None)": 0.009055123633314255, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.17590535300444554, "'production of IV sets' (unit, RER, None)": 2.1990013469576892, "'medical connector' (unit, GLO, None)": 0.39938175571307044, "'market for sodium chlorate, powder' (kilogram, RER, None)": 5.148719634703583e-06, "'stopcock' (unit, GLO, None)": 0.3250128508974576, "'market for water, ultrapure' (kilogram, RER, None)": 0.0071218718989447885, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.059513972203317125}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.005681742887412791, "'packed box of penicillin' (unit, SE, None)": 0.4107404572756075, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.383308540288312e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.9544240647015759, "'full box of vials' (unit, NO, None)": 0.3571104942253917, "'production of gloves' (unit, MY, None)": 0.00397044706317054, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0018484501955930203, "'production of IV sets' (unit, RER, None)": 0.20887798199967178, "'medical connector' (unit, GLO, None)": 0.03551769074884779, "'market for sodium chlorate, powder' (kilogram, RER, None)": 4.1827803350125506e-07, "'stopcock' (unit, GLO, None)": 0.02141764497794181, "'market for water, ultrapure' (kilogram, RER, None)": 0.0006153625812945318, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00223030389672603}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0002834639472163681, "'packed box of penicillin' (unit, SE, None)": 0.11903683140846391, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.0450216670264861e-05}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.8867178454987492, "'full box of vials' (unit, NO, None)": 0.02176082778009882, "'production of gloves' (unit, MY, None)": 0.00021512640371472653, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.000948280859940274, "'production of IV sets' (unit, RER, None)": 0.33261922330544524, "'medical connector' (unit, GLO, None)": 0.018670347089575857, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.9288147293366414e-06, "'stopcock' (unit, GLO, None)": 0.030079793081911083, "'market for water, ultrapure' (kilogram, RER, None)": 0.00021113546013968885, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0005977400582210082}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.00026335520011312854, "'packed box of penicillin' (unit, SE, None)": 0.00725360926003294, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.662126945771603e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.25418916593008745, "'full box of vials' (unit, NO, None)": 0.040778162362854455, "'production of gloves' (unit, MY, None)": 0.00020929931702298992, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.001444586756887401, "'production of IV sets' (unit, RER, None)": 0.06302993413100622, "'medical connector' (unit, GLO, None)": 0.01465675552791771, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.6809075394952411e-06, "'stopcock' (unit, GLO, None)": 0.02309867442366211, "'market for water, ultrapure' (kilogram, RER, None)": 0.00016647667404630034, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.002361076938021631}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 7.549418228123598e-05, "'packed box of penicillin' (unit, SE, None)": 0.013592720787618152, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.508758024045095e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 4.534613583951555e-06, "'full box of vials' (unit, NO, None)": 3.1914881829874047e-07, "'production of gloves' (unit, MY, None)": 3.8342036009936194e-09, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.2070602024453945e-08, "'production of IV sets' (unit, RER, None)": 3.4442983011362307e-06, "'medical connector' (unit, GLO, None)": 1.832767242754516e-07, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.2306374555740777e-12, "'stopcock' (unit, GLO, None)": 9.169736687692799e-08, "'market for water, ultrapure' (kilogram, RER, None)": 2.480877871327275e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.989283198447722e-08}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.346780234433612e-09, "'packed box of penicillin' (unit, SE, None)": 1.0638293943291351e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.0091623877815206e-11}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.01570731896700782, "'full box of vials' (unit, NO, None)": 0.0009952287770433926, "'production of gloves' (unit, MY, None)": 1.0564783297296858e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 9.323734333854125e-05, "'production of IV sets' (unit, RER, None)": 0.002820737018573794, "'medical connector' (unit, GLO, None)": 0.0007940186047471415, "'market for sodium chlorate, powder' (kilogram, RER, None)": 9.087066504422402e-09, "'stopcock' (unit, GLO, None)": 0.0005910881915482605, "'market for water, ultrapure' (kilogram, RER, None)": 1.3611427443396664e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.663304958430372e-05}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 4.6650737332013236e-06, "'packed box of penicillin' (unit, SE, None)": 0.0003317429256811309, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.780650963848533e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.028469902593481512, "'full box of vials' (unit, NO, None)": 0.0013267250712529284, "'production of gloves' (unit, MY, None)": 1.4163530975786153e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00013038775144206985, "'production of IV sets' (unit, RER, None)": 0.005329103349090954, "'medical connector' (unit, GLO, None)": 0.0013055374386428968, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.4313303962684281e-08, "'stopcock' (unit, GLO, None)": 0.0012081589085005972, "'market for water, ultrapure' (kilogram, RER, None)": 2.1482829273697714e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011138873995824629}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 8.45556107026401e-06, "'packed box of penicillin' (unit, SE, None)": 0.0004422416904176429, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.727841352826915e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.029320884509801824, "'full box of vials' (unit, NO, None)": 0.001370266861425661, "'production of gloves' (unit, MY, None)": 1.4684859631314947e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.00013398816890110104, "'production of IV sets' (unit, RER, None)": 0.0056220500711255126, "'medical connector' (unit, GLO, None)": 0.0013874429068758327, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.5185667717271498e-08, "'stopcock' (unit, GLO, None)": 0.00129525752812853, "'market for water, ultrapure' (kilogram, RER, None)": 2.301058855254493e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011945921458723627}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 8.708302699411142e-06, "'packed box of penicillin' (unit, SE, None)": 0.00045675562047522034, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.865055054962094e-08}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.0984780181258722, "'full box of vials' (unit, NO, None)": 0.03600192407055957, "'production of gloves' (unit, MY, None)": 0.0003173932895559447, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0004300178534555128, "'production of IV sets' (unit, RER, None)": 0.06342684359841966, "'medical connector' (unit, GLO, None)": 0.006814612431333982, "'market for sodium chlorate, powder' (kilogram, RER, None)": 8.352207092016413e-08, "'stopcock' (unit, GLO, None)": 0.0045883152102746995, "'market for water, ultrapure' (kilogram, RER, None)": 0.00011038760144267684, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0005103083642199823}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 2.924797138338405e-05, "'packed box of penicillin' (unit, SE, None)": 0.01200064135685319, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -8.353791381112465e-07}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 4.902932398442658e-08, "'full box of vials' (unit, NO, None)": 3.250424588023479e-09, "'production of gloves' (unit, MY, None)": 1.255259533483824e-10, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 2.2394392106546851e-10, "'production of IV sets' (unit, RER, None)": 1.3283534486921163e-08, "'medical connector' (unit, GLO, None)": 2.5510225773413464e-09, "'market for sodium chlorate, powder' (kilogram, RER, None)": 3.994779346027959e-14, "'stopcock' (unit, GLO, None)": 1.7036204159597961e-09, "'market for water, ultrapure' (kilogram, RER, None)": 4.054206414751791e-11, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.99334950990401e-10}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 1.4561709223374696e-11, "'packed box of penicillin' (unit, SE, None)": 1.083474862674493e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.303843092129425e-13}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 2.633485617414525e-05, "'full box of vials' (unit, NO, None)": 2.050867868836324e-06, "'production of gloves' (unit, MY, None)": 2.215139896920989e-08, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 1.6379692023869563e-07, "'production of IV sets' (unit, RER, None)": 5.217602017801188e-06, "'medical connector' (unit, GLO, None)": 1.2608984953567032e-06, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.2980902065251225e-11, "'stopcock' (unit, GLO, None)": 8.112728205819187e-07, "'market for water, ultrapure' (kilogram, RER, None)": 2.1009379318096128e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.4476942110326793e-07}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 7.82145228372114e-09, "'packed box of penicillin' (unit, SE, None)": 6.836226229454415e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.830248208696044e-11}</t>
-  </si>
-  <si>
-    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.7962346041941827, "'full box of vials' (unit, NO, None)": 0.048278798871591394, "'production of gloves' (unit, MY, None)": 0.00047405597484428193, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": 0.0037737425754329895, "'production of IV sets' (unit, RER, None)": 0.23871495679333327, "'medical connector' (unit, GLO, None)": 0.10451083724522091, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.2485945693722554e-06, "'stopcock' (unit, GLO, None)": 0.06860538337334873, "'market for water, ultrapure' (kilogram, RER, None)": 0.0015021057997467893, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.006191267771795764}</t>
-  </si>
-  <si>
-    <t>{"'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": 0.0002364816774456723, "'packed box of penicillin' (unit, SE, None)": 0.01609293295719713, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.2477153257901502e-06}</t>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.024388112839793738, "'packaging of glass vials with penicillin G' (unit, NO, None)": 2.548765915624195e-06, "'production of a pair of gloves' (unit, MY, None)": 0.0016420437097753881, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.0016700908863142114, "'production of IV sets' (unit, RER, None)": 0.008454665850606434, "'medical connector' (unit, GLO, None)": 0.0017344477364648202, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.3883780810126298e-06, "'stopcock' (unit, GLO, None)": 2.0100951733444598e-05, "'market for water, ultrapure' (kilogram, RER, None)": 2.8267764292293542e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00012390267575063623}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.0008129370946597914, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -7.56983476940386e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.321859044128822e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 6.797642744924298, "'packaging of glass vials with penicillin G' (unit, NO, None)": 0.0007824541369516421, "'production of a pair of gloves' (unit, MY, None)": 0.334228589000505, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.7091342106453968, "'production of IV sets' (unit, RER, None)": 2.475546646547223, "'medical connector' (unit, GLO, None)": 0.6079081956249768, "'market for sodium chlorate, powder' (kilogram, RER, None)": 0.0003964233839754639, "'stopcock' (unit, GLO, None)": 0.006091395717158148, "'market for water, ultrapure' (kilogram, RER, None)": 0.009729568585083915, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.15039954421117394}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.2265880914974766, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -2.323888786746377e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0008796896462493291}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.5388704942220609, "'packaging of glass vials with penicillin G' (unit, NO, None)": 3.374330432330913e-05, "'production of a pair of gloves' (unit, MY, None)": 0.07596319064128952, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.03946832670683045, "'production of IV sets' (unit, RER, None)": 0.1459841640314835, "'medical connector' (unit, GLO, None)": 0.018047961482087045, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.3411141316876487e-05, "'stopcock' (unit, GLO, None)": 0.0002022736050311023, "'market for water, ultrapure' (kilogram, RER, None)": 0.00033203580738642746, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0025378134464491137}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.017962349807402033, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -1.0021761384022811e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00019993511776787403}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.7095240446617761, "'packaging of glass vials with penicillin G' (unit, NO, None)": 4.496894699166291e-05, "'production of a pair of gloves' (unit, MY, None)": 0.11239164794124026, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.05109291850979622, "'production of IV sets' (unit, RER, None)": 0.18231620677928956, "'medical connector' (unit, GLO, None)": 0.023746813887832785, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.8036422689467295e-05, "'stopcock' (unit, GLO, None)": 0.0002685430926629082, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004282569032831853, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.003462827122704726}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.02365080148872587, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -1.3355777256523883e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0002958148173813444}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 26.45432784299862, "'packaging of glass vials with penicillin G' (unit, NO, None)": 0.001660728443221792, "'production of a pair of gloves' (unit, MY, None)": 2.7410492691807877, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -2.629682145382761, "'production of IV sets' (unit, RER, None)": 11.664008279678415, "'medical connector' (unit, GLO, None)": 1.6751476452045957, "'market for sodium chlorate, powder' (kilogram, RER, None)": 0.0011500389037977557, "'stopcock' (unit, GLO, None)": 0.01968370828069925, "'market for water, ultrapure' (kilogram, RER, None)": 0.03075217768355013, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.1386216181064803}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.881810928099954, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -4.932363476368722e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.007214441676483834}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.821712731969444, "'packaging of glass vials with penicillin G' (unit, NO, None)": 0.00020180203363117557, "'production of a pair of gloves' (unit, MY, None)": 0.09671491966461047, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.17326802795323423, "'production of IV sets' (unit, RER, None)": 0.6085899750643082, "'medical connector' (unit, GLO, None)": 0.28547008978087873, "'market for sodium chlorate, powder' (kilogram, RER, None)": 0.00021874585199251615, "'stopcock' (unit, GLO, None)": 0.002724599880413149, "'market for water, ultrapure' (kilogram, RER, None)": 0.004298967283073772, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.015032573771397403}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.0607237577323148, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -5.993520398845915e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0002545536685572548}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.00574742611515957, "'packaging of glass vials with penicillin G' (unit, NO, None)": 1.4021999709873185e-05, "'production of a pair of gloves' (unit, MY, None)": 0.00018922433751518717, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.00021567686243347206, "'production of IV sets' (unit, RER, None)": 0.0011125325403913585, "'medical connector' (unit, GLO, None)": 0.00015211175421089626, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.1452973084879706e-07, "'stopcock' (unit, GLO, None)": 2.222299054210985e-06, "'market for water, ultrapure' (kilogram, RER, None)": 2.732997898108185e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.1034570663069486e-05}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.000191580870505319, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -4.164533913832336e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.980384563399727e-07}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.0006246461383110954, "'packaging of glass vials with penicillin G' (unit, NO, None)": 1.9211096379213993e-06, "'production of a pair of gloves' (unit, MY, None)": 1.0680528176019501e-05, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.00012983417071484144, "'production of IV sets' (unit, RER, None)": 0.0006357027536749809, "'medical connector' (unit, GLO, None)": 2.0791331621824976e-05, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.652238343114176e-08, "'stopcock' (unit, GLO, None)": 8.367926170619175e-07, "'market for water, ultrapure' (kilogram, RER, None)": 3.221977583310162e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.2595014347319692e-06}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 2.0821537943703183e-05, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -5.705695624626555e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.811115015928333e-08}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 1.2938265065462826, "'packaging of glass vials with penicillin G' (unit, NO, None)": 0.00016372748895885543, "'production of a pair of gloves' (unit, MY, None)": 0.05310275329465476, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.029119097358752406, "'production of IV sets' (unit, RER, None)": 0.13167305838088722, "'medical connector' (unit, GLO, None)": 0.027135028888640812, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.8729109246335604e-05, "'stopcock' (unit, GLO, None)": 0.00026959855560932565, "'market for water, ultrapure' (kilogram, RER, None)": 0.0004616459759680086, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.016495415108423565}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.04312755021820942, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -4.862706422078006e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00013976644667153132}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 12.322213950685356, "'packaging of glass vials with penicillin G' (unit, NO, None)": 0.0009055127891084376, "'production of a pair of gloves' (unit, MY, None)": 1.336869991085971, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.60508780310318, "'production of IV sets' (unit, RER, None)": 2.659367113894098, "'medical connector' (unit, GLO, None)": 0.39938176713543566, "'market for sodium chlorate, powder' (kilogram, RER, None)": 0.0003306303359861266, "'stopcock' (unit, GLO, None)": 0.005720799627692931, "'market for water, ultrapure' (kilogram, RER, None)": 0.007121871899215062, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.05951397515972752}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.4107404650228452, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -2.68937298365206e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0035186418165382757}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 3.5711049594139617, "'packaging of glass vials with penicillin G' (unit, NO, None)": 0.00039704470944142015, "'production of a pair of gloves' (unit, MY, None)": 0.014048109233323083, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.09425926094275014, "'production of IV sets' (unit, RER, None)": 0.47695633783002966, "'medical connector' (unit, GLO, None)": 0.03551769075980439, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.9581954635774115e-05, "'stopcock' (unit, GLO, None)": 0.000464753372131344, "'market for water, ultrapure' (kilogram, RER, None)": 0.0006153625809124813, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0022303039216704933}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.1190368319804654, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -1.1792227870410178e-06, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.697462350210635e-05}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.21760830117477667, "'packaging of glass vials with penicillin G' (unit, NO, None)": 2.151265093169469e-05, "'production of a pair of gloves' (unit, MY, None)": 0.007206876909437653, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.07358582375551662, "'production of IV sets' (unit, RER, None)": 0.3441222366986121, "'medical connector' (unit, GLO, None)": 0.01867034693696131, "'market for sodium chlorate, powder' (kilogram, RER, None)": 4.132522978566995e-05, "'stopcock' (unit, GLO, None)": 0.0021431274781735987, "'market for water, ultrapure' (kilogram, RER, None)": 0.00021113547721983515, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.000597740172076272}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.0072536100391592225, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -6.389257326713324e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.89685000256399e-05}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.40778163777727716, "'packaging of glass vials with penicillin G' (unit, NO, None)": 2.0929934841080258e-05, "'production of a pair of gloves' (unit, MY, None)": 0.010978771539946868, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.013004013519171173, "'production of IV sets' (unit, RER, None)": 0.061287112432552526, "'medical connector' (unit, GLO, None)": 0.014656755502129009, "'market for sodium chlorate, powder' (kilogram, RER, None)": 6.17841627341382e-06, "'stopcock' (unit, GLO, None)": 0.0018676750452771623, "'market for water, ultrapure' (kilogram, RER, None)": 0.00016647667143573455, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0023610769331310682}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.013592721259242572, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -6.216190647800837e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.889612669314016e-05}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 3.191488238990637e-06, "'packaging of glass vials with penicillin G' (unit, NO, None)": 3.8342037086440855e-10, "'production of a pair of gloves' (unit, MY, None)": 9.173584167505032e-08, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -4.784810839071028e-07, "'production of IV sets' (unit, RER, None)": 3.423098271384921e-06, "'medical connector' (unit, GLO, None)": 1.832767241169912e-07, "'market for sodium chlorate, powder' (kilogram, RER, None)": 8.679671987789016e-11, "'stopcock' (unit, GLO, None)": 2.478486066524837e-09, "'market for water, ultrapure' (kilogram, RER, None)": 2.480877861057824e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.989283214660891e-08}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 1.0638294129968791e-07, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -1.1387585014672934e-12, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.4144873528873244e-10}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.009952288119191757, "'packaging of glass vials with penicillin G' (unit, NO, None)": 1.0564784720953878e-06, "'production of a pair of gloves' (unit, MY, None)": 0.000708598141510353, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.0006573703490751319, "'production of IV sets' (unit, RER, None)": 0.0032287110653313, "'medical connector' (unit, GLO, None)": 0.0007940186068696452, "'market for sodium chlorate, powder' (kilogram, RER, None)": 6.056776235331688e-07, "'stopcock' (unit, GLO, None)": 1.0096740593826251e-05, "'market for water, ultrapure' (kilogram, RER, None)": 1.3611427403493864e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -5.663305084383919e-05}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.0003317429373063919, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -3.1377410621233016e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -1.865030308455249e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.013267251309552093, "'packaging of glass vials with penicillin G' (unit, NO, None)": 1.4163531581966652e-06, "'production of a pair of gloves' (unit, MY, None)": 0.0009909389824058704, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.0011905610474030625, "'production of IV sets' (unit, RER, None)": 0.0054121406006530535, "'medical connector' (unit, GLO, None)": 0.001305537435978577, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.1983734411714549e-06, "'stopcock' (unit, GLO, None)": 1.5903671116318822e-05, "'market for water, ultrapure' (kilogram, RER, None)": 2.1482829243264233e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011138874214759248}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.0004422417103184032, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -4.206568879844096e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.608151401692251e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.013702669236096346, "'packaging of glass vials with penicillin G' (unit, NO, None)": 1.4684860272501623e-06, "'production of a pair of gloves' (unit, MY, None)": 0.0010183019361641738, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.001255722252517463, "'production of IV sets' (unit, RER, None)": 0.005645151610380906, "'medical connector' (unit, GLO, None)": 0.0013874429037551259, "'market for sodium chlorate, powder' (kilogram, RER, None)": 1.2920439862929296e-06, "'stopcock' (unit, GLO, None)": 1.6872964181181785e-05, "'market for water, ultrapure' (kilogram, RER, None)": 2.3010588520399164e-05, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.00011945921703611581}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.00045675564120321155, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -4.361403500932982e-09, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.6801706959841056e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.36001924167002103, "'packaging of glass vials with penicillin G' (unit, NO, None)": 3.17393292549663e-05, "'production of a pair of gloves' (unit, MY, None)": 0.0032681095434796466, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.008938155779947513, "'production of IV sets' (unit, RER, None)": 0.06669587453670975, "'medical connector' (unit, GLO, None)": 0.0068146124300296675, "'market for sodium chlorate, powder' (kilogram, RER, None)": 4.739050439188589e-06, "'stopcock' (unit, GLO, None)": 9.280230109423735e-05, "'market for water, ultrapure' (kilogram, RER, None)": 0.00011038760116389587, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.0005103083655294562}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.0120006413890007, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -9.426580788724992e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -8.60166431843843e-06}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 3.2504246804574604e-08, "'packaging of glass vials with penicillin G' (unit, NO, None)": 1.2552595704719405e-11, "'production of a pair of gloves' (unit, MY, None)": 1.7019601865468382e-09, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -3.362140150295813e-09, "'production of IV sets' (unit, RER, None)": 1.350678088406866e-08, "'medical connector' (unit, GLO, None)": 2.5510225775175463e-09, "'market for sodium chlorate, powder' (kilogram, RER, None)": 2.0388603300629357e-12, "'stopcock' (unit, GLO, None)": 4.4386437253703525e-11, "'market for water, ultrapure' (kilogram, RER, None)": 4.0542064206491157e-11, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.993349548382644e-10}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 1.08347489348582e-09, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -3.728120924301663e-14, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -4.479559210991278e-12}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 2.0508679353033688e-05, "'packaging of glass vials with penicillin G' (unit, NO, None)": 2.215140165251004e-09, "'production of a pair of gloves' (unit, MY, None)": 1.2448466369579436e-06, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -1.327754741714953e-06, "'production of IV sets' (unit, RER, None)": 5.528568489056439e-06, "'medical connector' (unit, GLO, None)": 1.260898497704189e-06, "'market for sodium chlorate, powder' (kilogram, RER, None)": 8.978371595674199e-10, "'stopcock' (unit, GLO, None)": 1.4423224579857376e-08, "'market for water, ultrapure' (kilogram, RER, None)": 2.100937923156657e-08, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -2.447694229653816e-07}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 6.83622645101123e-07, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -6.578966290795481e-12, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -3.2764363484733075e-09}</t>
+  </si>
+  <si>
+    <t>{"'production of alchohol wipes' (unit, DK, None)": 0.48278800341591116, "'packaging of glass vials with penicillin G' (unit, NO, None)": 4.740560014392543e-05, "'production of a pair of gloves' (unit, MY, None)": 0.028680214153030546, "'treatment of hazardous waste, hazardous waste incineration, with energy recovery' (kilogram, CH, None)": -0.058473024972178454, "'production of IV sets' (unit, RER, None)": 0.19276334332556483, "'medical connector' (unit, GLO, None)": 0.10451083715028212, "'market for sodium chlorate, powder' (kilogram, RER, None)": 8.459359061438786e-05, "'stopcock' (unit, GLO, None)": 0.0013873273007062794, "'market for water, ultrapure' (kilogram, RER, None)": 0.001502105798808324, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -0.006191267833945877}</t>
+  </si>
+  <si>
+    <t>{"'packed box of penicillin' (unit, SE, None)": 0.01609293344719704, "'treatment of hazardous waste, hazardous waste incineration' (kilogram, CH, None)": -1.4079463242745854e-07, "'waste packaging paper, Recycled Content cut-off' (kilogram, GLO, None)": -7.54863236507764e-05}</t>
   </si>
 </sst>
 </file>

</xml_diff>